<commit_message>
updated results and code
</commit_message>
<xml_diff>
--- a/stats/avey/disease_type=all failure-type-ignored=None for app=NA.xlsx
+++ b/stats/avey/disease_type=all failure-type-ignored=None for app=NA.xlsx
@@ -970,13 +970,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.401</v>
+        <v>0.402</v>
       </c>
       <c r="C4" t="n">
-        <v>0.079</v>
+        <v>0.078</v>
       </c>
       <c r="D4" t="n">
-        <v>0.281</v>
+        <v>0.279</v>
       </c>
       <c r="E4" t="n">
         <v>0.446</v>
@@ -985,28 +985,28 @@
         <v>0.073</v>
       </c>
       <c r="G4" t="n">
-        <v>0.271</v>
+        <v>0.27</v>
       </c>
       <c r="H4" t="n">
-        <v>0.38</v>
+        <v>0.382</v>
       </c>
       <c r="I4" t="n">
         <v>0.068</v>
       </c>
       <c r="J4" t="n">
-        <v>0.261</v>
+        <v>0.26</v>
       </c>
       <c r="K4" t="n">
         <v>0.395</v>
       </c>
       <c r="L4" t="n">
-        <v>0.062</v>
+        <v>0.061</v>
       </c>
       <c r="M4" t="n">
-        <v>0.249</v>
+        <v>0.247</v>
       </c>
       <c r="N4" t="n">
-        <v>0.442</v>
+        <v>0.444</v>
       </c>
       <c r="O4" t="n">
         <v>0.068</v>
@@ -1015,13 +1015,13 @@
         <v>0.261</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.037</v>
+        <v>0.036</v>
       </c>
       <c r="R4" t="n">
         <v>0.033</v>
       </c>
       <c r="S4" t="n">
-        <v>0.183</v>
+        <v>0.181</v>
       </c>
       <c r="T4" t="n">
         <v>0.344</v>
@@ -1033,16 +1033,16 @@
         <v>0.335</v>
       </c>
       <c r="W4" t="n">
-        <v>0.3</v>
+        <v>0.298</v>
       </c>
       <c r="X4" t="n">
         <v>0.111</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.334</v>
+        <v>0.333</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.374</v>
+        <v>0.373</v>
       </c>
       <c r="AA4" t="n">
         <v>0.063</v>
@@ -1051,13 +1051,13 @@
         <v>0.252</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.471</v>
+        <v>0.472</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.22</v>
+        <v>0.221</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.469</v>
+        <v>0.47</v>
       </c>
       <c r="AF4" t="n">
         <v>0.256</v>
@@ -1066,19 +1066,19 @@
         <v>0.092</v>
       </c>
       <c r="AH4" t="n">
-        <v>0.303</v>
+        <v>0.304</v>
       </c>
       <c r="AI4" t="n">
-        <v>0.315</v>
+        <v>0.313</v>
       </c>
       <c r="AJ4" t="n">
-        <v>0.098</v>
+        <v>0.097</v>
       </c>
       <c r="AK4" t="n">
-        <v>0.313</v>
+        <v>0.312</v>
       </c>
       <c r="AL4" t="n">
-        <v>0.281</v>
+        <v>0.283</v>
       </c>
       <c r="AM4" t="n">
         <v>0.083</v>
@@ -1087,7 +1087,7 @@
         <v>0.288</v>
       </c>
       <c r="AO4" t="n">
-        <v>0.506</v>
+        <v>0.508</v>
       </c>
       <c r="AP4" t="n">
         <v>0.155</v>
@@ -1096,16 +1096,16 @@
         <v>0.394</v>
       </c>
       <c r="AR4" t="n">
-        <v>0.181</v>
+        <v>0.18</v>
       </c>
       <c r="AS4" t="n">
         <v>0.029</v>
       </c>
       <c r="AT4" t="n">
-        <v>0.17</v>
+        <v>0.169</v>
       </c>
       <c r="AU4" t="n">
-        <v>0.215</v>
+        <v>0.217</v>
       </c>
       <c r="AV4" t="n">
         <v>0.03</v>
@@ -1114,34 +1114,34 @@
         <v>0.174</v>
       </c>
       <c r="AX4" t="n">
-        <v>2.13</v>
+        <v>2.137</v>
       </c>
       <c r="AY4" t="n">
         <v>0.148</v>
       </c>
       <c r="AZ4" t="n">
-        <v>0.385</v>
+        <v>0.384</v>
       </c>
       <c r="BA4" t="n">
         <v>2.086</v>
       </c>
       <c r="BB4" t="n">
-        <v>0.155</v>
+        <v>0.153</v>
       </c>
       <c r="BC4" t="n">
-        <v>0.394</v>
+        <v>0.392</v>
       </c>
       <c r="BD4" t="n">
-        <v>0.782</v>
+        <v>0.784</v>
       </c>
       <c r="BE4" t="n">
-        <v>0.122</v>
+        <v>0.121</v>
       </c>
       <c r="BF4" t="n">
-        <v>0.349</v>
+        <v>0.347</v>
       </c>
       <c r="BG4" t="n">
-        <v>0.782</v>
+        <v>0.78</v>
       </c>
       <c r="BH4" t="n">
         <v>0.123</v>
@@ -1150,10 +1150,10 @@
         <v>0.351</v>
       </c>
       <c r="BJ4" t="n">
-        <v>0.751</v>
+        <v>0.753</v>
       </c>
       <c r="BK4" t="n">
-        <v>0.078</v>
+        <v>0.077</v>
       </c>
       <c r="BL4" t="n">
         <v>0.278</v>
@@ -1162,16 +1162,16 @@
         <v>0.719</v>
       </c>
       <c r="BN4" t="n">
-        <v>0.08599999999999999</v>
+        <v>0.08500000000000001</v>
       </c>
       <c r="BO4" t="n">
-        <v>0.293</v>
+        <v>0.292</v>
       </c>
       <c r="BP4" t="n">
         <v>0.695</v>
       </c>
       <c r="BQ4" t="n">
-        <v>0.71</v>
+        <v>0.712</v>
       </c>
     </row>
     <row r="5">
@@ -1181,13 +1181,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.5</v>
+        <v>0.501</v>
       </c>
       <c r="C5" t="n">
-        <v>0.093</v>
+        <v>0.092</v>
       </c>
       <c r="D5" t="n">
-        <v>0.305</v>
+        <v>0.303</v>
       </c>
       <c r="E5" t="n">
         <v>0.589</v>
@@ -1199,7 +1199,7 @@
         <v>0.297</v>
       </c>
       <c r="H5" t="n">
-        <v>0.591</v>
+        <v>0.595</v>
       </c>
       <c r="I5" t="n">
         <v>0.126</v>
@@ -1208,31 +1208,31 @@
         <v>0.355</v>
       </c>
       <c r="K5" t="n">
-        <v>0.626</v>
+        <v>0.628</v>
       </c>
       <c r="L5" t="n">
-        <v>0.116</v>
+        <v>0.115</v>
       </c>
       <c r="M5" t="n">
-        <v>0.34</v>
+        <v>0.339</v>
       </c>
       <c r="N5" t="n">
-        <v>0.736</v>
+        <v>0.739</v>
       </c>
       <c r="O5" t="n">
         <v>0.078</v>
       </c>
       <c r="P5" t="n">
-        <v>0.28</v>
+        <v>0.279</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.022</v>
+        <v>0.021</v>
       </c>
       <c r="R5" t="n">
-        <v>0.014</v>
+        <v>0.013</v>
       </c>
       <c r="S5" t="n">
-        <v>0.117</v>
+        <v>0.116</v>
       </c>
       <c r="T5" t="n">
         <v>0.314</v>
@@ -1244,16 +1244,16 @@
         <v>0.307</v>
       </c>
       <c r="W5" t="n">
-        <v>0.293</v>
+        <v>0.291</v>
       </c>
       <c r="X5" t="n">
-        <v>0.107</v>
+        <v>0.106</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.327</v>
+        <v>0.326</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.511</v>
+        <v>0.508</v>
       </c>
       <c r="AA5" t="n">
         <v>0.104</v>
@@ -1262,16 +1262,16 @@
         <v>0.322</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.231</v>
+        <v>0.23</v>
       </c>
       <c r="AD5" t="n">
         <v>0.059</v>
       </c>
       <c r="AE5" t="n">
-        <v>0.243</v>
+        <v>0.242</v>
       </c>
       <c r="AF5" t="n">
-        <v>0.259</v>
+        <v>0.258</v>
       </c>
       <c r="AG5" t="n">
         <v>0.08500000000000001</v>
@@ -1280,16 +1280,16 @@
         <v>0.292</v>
       </c>
       <c r="AI5" t="n">
-        <v>0.353</v>
+        <v>0.35</v>
       </c>
       <c r="AJ5" t="n">
         <v>0.114</v>
       </c>
       <c r="AK5" t="n">
-        <v>0.338</v>
+        <v>0.337</v>
       </c>
       <c r="AL5" t="n">
-        <v>0.368</v>
+        <v>0.372</v>
       </c>
       <c r="AM5" t="n">
         <v>0.118</v>
@@ -1307,52 +1307,52 @@
         <v>0.287</v>
       </c>
       <c r="AR5" t="n">
-        <v>0.432</v>
+        <v>0.431</v>
       </c>
       <c r="AS5" t="n">
+        <v>0.109</v>
+      </c>
+      <c r="AT5" t="n">
+        <v>0.331</v>
+      </c>
+      <c r="AU5" t="n">
+        <v>0.444</v>
+      </c>
+      <c r="AV5" t="n">
         <v>0.11</v>
       </c>
-      <c r="AT5" t="n">
+      <c r="AW5" t="n">
         <v>0.332</v>
       </c>
-      <c r="AU5" t="n">
-        <v>0.441</v>
-      </c>
-      <c r="AV5" t="n">
-        <v>0.111</v>
-      </c>
-      <c r="AW5" t="n">
-        <v>0.333</v>
-      </c>
       <c r="AX5" t="n">
-        <v>1.368</v>
+        <v>1.37</v>
       </c>
       <c r="AY5" t="n">
-        <v>0.07099999999999999</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="AZ5" t="n">
-        <v>0.266</v>
+        <v>0.265</v>
       </c>
       <c r="BA5" t="n">
-        <v>1.398</v>
+        <v>1.397</v>
       </c>
       <c r="BB5" t="n">
-        <v>0.078</v>
+        <v>0.077</v>
       </c>
       <c r="BC5" t="n">
-        <v>0.279</v>
+        <v>0.277</v>
       </c>
       <c r="BD5" t="n">
-        <v>0.4</v>
+        <v>0.399</v>
       </c>
       <c r="BE5" t="n">
-        <v>0.043</v>
+        <v>0.042</v>
       </c>
       <c r="BF5" t="n">
-        <v>0.207</v>
+        <v>0.205</v>
       </c>
       <c r="BG5" t="n">
-        <v>0.413</v>
+        <v>0.412</v>
       </c>
       <c r="BH5" t="n">
         <v>0.049</v>
@@ -1361,13 +1361,13 @@
         <v>0.222</v>
       </c>
       <c r="BJ5" t="n">
-        <v>0.556</v>
+        <v>0.5580000000000001</v>
       </c>
       <c r="BK5" t="n">
         <v>0.058</v>
       </c>
       <c r="BL5" t="n">
-        <v>0.241</v>
+        <v>0.242</v>
       </c>
       <c r="BM5" t="n">
         <v>0.573</v>
@@ -1376,13 +1376,13 @@
         <v>0.067</v>
       </c>
       <c r="BO5" t="n">
-        <v>0.259</v>
+        <v>0.258</v>
       </c>
       <c r="BP5" t="n">
         <v>0.466</v>
       </c>
       <c r="BQ5" t="n">
-        <v>0.456</v>
+        <v>0.457</v>
       </c>
     </row>
     <row r="6">
@@ -1392,7 +1392,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.445</v>
+        <v>0.446</v>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
@@ -1402,22 +1402,22 @@
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="n">
-        <v>0.463</v>
+        <v>0.465</v>
       </c>
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="n">
-        <v>0.484</v>
+        <v>0.485</v>
       </c>
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="n">
-        <v>0.552</v>
+        <v>0.555</v>
       </c>
       <c r="O6" t="inlineStr"/>
       <c r="P6" t="inlineStr"/>
       <c r="Q6" t="n">
-        <v>0.028</v>
+        <v>0.027</v>
       </c>
       <c r="R6" t="inlineStr"/>
       <c r="S6" t="inlineStr"/>
@@ -1427,17 +1427,17 @@
       <c r="U6" t="inlineStr"/>
       <c r="V6" t="inlineStr"/>
       <c r="W6" t="n">
-        <v>0.296</v>
+        <v>0.294</v>
       </c>
       <c r="X6" t="inlineStr"/>
       <c r="Y6" t="inlineStr"/>
       <c r="Z6" t="n">
-        <v>0.432</v>
+        <v>0.43</v>
       </c>
       <c r="AA6" t="inlineStr"/>
       <c r="AB6" t="inlineStr"/>
       <c r="AC6" t="n">
-        <v>0.31</v>
+        <v>0.309</v>
       </c>
       <c r="AD6" t="inlineStr"/>
       <c r="AE6" t="inlineStr"/>
@@ -1447,12 +1447,12 @@
       <c r="AG6" t="inlineStr"/>
       <c r="AH6" t="inlineStr"/>
       <c r="AI6" t="n">
-        <v>0.333</v>
+        <v>0.33</v>
       </c>
       <c r="AJ6" t="inlineStr"/>
       <c r="AK6" t="inlineStr"/>
       <c r="AL6" t="n">
-        <v>0.319</v>
+        <v>0.321</v>
       </c>
       <c r="AM6" t="inlineStr"/>
       <c r="AN6" t="inlineStr"/>
@@ -1462,22 +1462,22 @@
       <c r="AP6" t="inlineStr"/>
       <c r="AQ6" t="inlineStr"/>
       <c r="AR6" t="n">
-        <v>0.255</v>
+        <v>0.254</v>
       </c>
       <c r="AS6" t="inlineStr"/>
       <c r="AT6" t="inlineStr"/>
       <c r="AU6" t="n">
-        <v>0.289</v>
+        <v>0.292</v>
       </c>
       <c r="AV6" t="inlineStr"/>
       <c r="AW6" t="inlineStr"/>
       <c r="AX6" t="n">
-        <v>1.656</v>
+        <v>1.659</v>
       </c>
       <c r="AY6" t="inlineStr"/>
       <c r="AZ6" t="inlineStr"/>
       <c r="BA6" t="n">
-        <v>1.662</v>
+        <v>1.661</v>
       </c>
       <c r="BB6" t="inlineStr"/>
       <c r="BC6" t="inlineStr"/>
@@ -1487,12 +1487,12 @@
       <c r="BE6" t="inlineStr"/>
       <c r="BF6" t="inlineStr"/>
       <c r="BG6" t="n">
-        <v>0.541</v>
+        <v>0.539</v>
       </c>
       <c r="BH6" t="inlineStr"/>
       <c r="BI6" t="inlineStr"/>
       <c r="BJ6" t="n">
-        <v>0.639</v>
+        <v>0.641</v>
       </c>
       <c r="BK6" t="inlineStr"/>
       <c r="BL6" t="inlineStr"/>
@@ -1505,7 +1505,7 @@
         <v>0.554</v>
       </c>
       <c r="BQ6" t="n">
-        <v>0.552</v>
+        <v>0.553</v>
       </c>
     </row>
     <row r="7">
@@ -1515,7 +1515,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.476</v>
+        <v>0.477</v>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
@@ -1525,22 +1525,22 @@
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="n">
-        <v>0.532</v>
+        <v>0.535</v>
       </c>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.5620000000000001</v>
       </c>
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="n">
-        <v>0.65</v>
+        <v>0.652</v>
       </c>
       <c r="O7" t="inlineStr"/>
       <c r="P7" t="inlineStr"/>
       <c r="Q7" t="n">
-        <v>0.024</v>
+        <v>0.023</v>
       </c>
       <c r="R7" t="inlineStr"/>
       <c r="S7" t="inlineStr"/>
@@ -1550,17 +1550,17 @@
       <c r="U7" t="inlineStr"/>
       <c r="V7" t="inlineStr"/>
       <c r="W7" t="n">
-        <v>0.294</v>
+        <v>0.292</v>
       </c>
       <c r="X7" t="inlineStr"/>
       <c r="Y7" t="inlineStr"/>
       <c r="Z7" t="n">
-        <v>0.476</v>
+        <v>0.474</v>
       </c>
       <c r="AA7" t="inlineStr"/>
       <c r="AB7" t="inlineStr"/>
       <c r="AC7" t="n">
-        <v>0.257</v>
+        <v>0.256</v>
       </c>
       <c r="AD7" t="inlineStr"/>
       <c r="AE7" t="inlineStr"/>
@@ -1570,12 +1570,12 @@
       <c r="AG7" t="inlineStr"/>
       <c r="AH7" t="inlineStr"/>
       <c r="AI7" t="n">
-        <v>0.345</v>
+        <v>0.342</v>
       </c>
       <c r="AJ7" t="inlineStr"/>
       <c r="AK7" t="inlineStr"/>
       <c r="AL7" t="n">
-        <v>0.347</v>
+        <v>0.35</v>
       </c>
       <c r="AM7" t="inlineStr"/>
       <c r="AN7" t="inlineStr"/>
@@ -1585,37 +1585,37 @@
       <c r="AP7" t="inlineStr"/>
       <c r="AQ7" t="inlineStr"/>
       <c r="AR7" t="n">
-        <v>0.338</v>
+        <v>0.337</v>
       </c>
       <c r="AS7" t="inlineStr"/>
       <c r="AT7" t="inlineStr"/>
       <c r="AU7" t="n">
-        <v>0.364</v>
+        <v>0.367</v>
       </c>
       <c r="AV7" t="inlineStr"/>
       <c r="AW7" t="inlineStr"/>
       <c r="AX7" t="n">
-        <v>1.468</v>
+        <v>1.47</v>
       </c>
       <c r="AY7" t="inlineStr"/>
       <c r="AZ7" t="inlineStr"/>
       <c r="BA7" t="n">
-        <v>1.491</v>
+        <v>1.49</v>
       </c>
       <c r="BB7" t="inlineStr"/>
       <c r="BC7" t="inlineStr"/>
       <c r="BD7" t="n">
-        <v>0.443</v>
+        <v>0.442</v>
       </c>
       <c r="BE7" t="inlineStr"/>
       <c r="BF7" t="inlineStr"/>
       <c r="BG7" t="n">
-        <v>0.456</v>
+        <v>0.455</v>
       </c>
       <c r="BH7" t="inlineStr"/>
       <c r="BI7" t="inlineStr"/>
       <c r="BJ7" t="n">
-        <v>0.586</v>
+        <v>0.588</v>
       </c>
       <c r="BK7" t="inlineStr"/>
       <c r="BL7" t="inlineStr"/>
@@ -1628,7 +1628,7 @@
         <v>0.497</v>
       </c>
       <c r="BQ7" t="n">
-        <v>0.489</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="8">
@@ -1638,16 +1638,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.543</v>
+        <v>0.544</v>
       </c>
       <c r="C8" t="n">
-        <v>0.116</v>
+        <v>0.115</v>
       </c>
       <c r="D8" t="n">
-        <v>0.341</v>
+        <v>0.339</v>
       </c>
       <c r="E8" t="n">
-        <v>0.637</v>
+        <v>0.636</v>
       </c>
       <c r="F8" t="n">
         <v>0.105</v>
@@ -1656,40 +1656,40 @@
         <v>0.324</v>
       </c>
       <c r="H8" t="n">
-        <v>0.618</v>
+        <v>0.621</v>
       </c>
       <c r="I8" t="n">
-        <v>0.129</v>
+        <v>0.128</v>
       </c>
       <c r="J8" t="n">
-        <v>0.359</v>
+        <v>0.357</v>
       </c>
       <c r="K8" t="n">
-        <v>0.673</v>
+        <v>0.676</v>
       </c>
       <c r="L8" t="n">
-        <v>0.112</v>
+        <v>0.111</v>
       </c>
       <c r="M8" t="n">
-        <v>0.334</v>
+        <v>0.333</v>
       </c>
       <c r="N8" t="n">
-        <v>0.778</v>
+        <v>0.78</v>
       </c>
       <c r="O8" t="n">
         <v>0.058</v>
       </c>
       <c r="P8" t="n">
-        <v>0.242</v>
+        <v>0.24</v>
       </c>
       <c r="Q8" t="n">
         <v>0.025</v>
       </c>
       <c r="R8" t="n">
-        <v>0.019</v>
+        <v>0.018</v>
       </c>
       <c r="S8" t="n">
-        <v>0.137</v>
+        <v>0.136</v>
       </c>
       <c r="T8" t="n">
         <v>0.364</v>
@@ -1701,7 +1701,7 @@
         <v>0.365</v>
       </c>
       <c r="W8" t="n">
-        <v>0.33</v>
+        <v>0.329</v>
       </c>
       <c r="X8" t="n">
         <v>0.138</v>
@@ -1710,13 +1710,13 @@
         <v>0.371</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.523</v>
+        <v>0.519</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.124</v>
+        <v>0.125</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.353</v>
+        <v>0.354</v>
       </c>
       <c r="AC8" t="n">
         <v>0.326</v>
@@ -1737,25 +1737,25 @@
         <v>0.341</v>
       </c>
       <c r="AI8" t="n">
-        <v>0.364</v>
+        <v>0.361</v>
       </c>
       <c r="AJ8" t="n">
-        <v>0.136</v>
+        <v>0.135</v>
       </c>
       <c r="AK8" t="n">
-        <v>0.369</v>
+        <v>0.368</v>
       </c>
       <c r="AL8" t="n">
-        <v>0.382</v>
+        <v>0.385</v>
       </c>
       <c r="AM8" t="n">
-        <v>0.138</v>
+        <v>0.137</v>
       </c>
       <c r="AN8" t="n">
         <v>0.371</v>
       </c>
       <c r="AO8" t="n">
-        <v>0.486</v>
+        <v>0.489</v>
       </c>
       <c r="AP8" t="n">
         <v>0.123</v>
@@ -1770,37 +1770,37 @@
         <v>0.106</v>
       </c>
       <c r="AT8" t="n">
-        <v>0.325</v>
+        <v>0.326</v>
       </c>
       <c r="AU8" t="n">
-        <v>0.399</v>
+        <v>0.402</v>
       </c>
       <c r="AV8" t="n">
-        <v>0.115</v>
+        <v>0.114</v>
       </c>
       <c r="AW8" t="n">
         <v>0.338</v>
       </c>
       <c r="AX8" t="n">
-        <v>1.841</v>
+        <v>1.844</v>
       </c>
       <c r="AY8" t="n">
-        <v>0.116</v>
+        <v>0.115</v>
       </c>
       <c r="AZ8" t="n">
-        <v>0.341</v>
+        <v>0.339</v>
       </c>
       <c r="BA8" t="n">
-        <v>1.839</v>
+        <v>1.84</v>
       </c>
       <c r="BB8" t="n">
-        <v>0.124</v>
+        <v>0.123</v>
       </c>
       <c r="BC8" t="n">
-        <v>0.352</v>
+        <v>0.351</v>
       </c>
       <c r="BD8" t="n">
-        <v>0.581</v>
+        <v>0.58</v>
       </c>
       <c r="BE8" t="n">
         <v>0.096</v>
@@ -1809,19 +1809,19 @@
         <v>0.31</v>
       </c>
       <c r="BG8" t="n">
-        <v>0.585</v>
+        <v>0.582</v>
       </c>
       <c r="BH8" t="n">
         <v>0.099</v>
       </c>
       <c r="BI8" t="n">
-        <v>0.314</v>
+        <v>0.315</v>
       </c>
       <c r="BJ8" t="n">
         <v>0.733</v>
       </c>
       <c r="BK8" t="n">
-        <v>0.052</v>
+        <v>0.051</v>
       </c>
       <c r="BL8" t="n">
         <v>0.227</v>
@@ -1833,13 +1833,13 @@
         <v>0.059</v>
       </c>
       <c r="BO8" t="n">
-        <v>0.244</v>
+        <v>0.242</v>
       </c>
       <c r="BP8" t="n">
         <v>0.613</v>
       </c>
       <c r="BQ8" t="n">
-        <v>0.614</v>
+        <v>0.615</v>
       </c>
     </row>
     <row r="9">
@@ -1849,16 +1849,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.441</v>
+        <v>0.439</v>
       </c>
       <c r="C9" t="n">
-        <v>0.247</v>
+        <v>0.246</v>
       </c>
       <c r="D9" t="n">
-        <v>0.497</v>
+        <v>0.496</v>
       </c>
       <c r="E9" t="n">
-        <v>0.546</v>
+        <v>0.543</v>
       </c>
       <c r="F9" t="n">
         <v>0.248</v>
@@ -1867,7 +1867,7 @@
         <v>0.498</v>
       </c>
       <c r="H9" t="n">
-        <v>0.525</v>
+        <v>0.526</v>
       </c>
       <c r="I9" t="n">
         <v>0.249</v>
@@ -1876,7 +1876,7 @@
         <v>0.499</v>
       </c>
       <c r="K9" t="n">
-        <v>0.609</v>
+        <v>0.61</v>
       </c>
       <c r="L9" t="n">
         <v>0.238</v>
@@ -1885,22 +1885,22 @@
         <v>0.488</v>
       </c>
       <c r="N9" t="n">
-        <v>0.6889999999999999</v>
+        <v>0.6909999999999999</v>
       </c>
       <c r="O9" t="n">
         <v>0.214</v>
       </c>
       <c r="P9" t="n">
-        <v>0.463</v>
+        <v>0.462</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.024</v>
+        <v>0.023</v>
       </c>
       <c r="R9" t="n">
         <v>0.023</v>
       </c>
       <c r="S9" t="n">
-        <v>0.152</v>
+        <v>0.151</v>
       </c>
       <c r="T9" t="n">
         <v>0.303</v>
@@ -1912,25 +1912,25 @@
         <v>0.46</v>
       </c>
       <c r="W9" t="n">
-        <v>0.269</v>
+        <v>0.268</v>
       </c>
       <c r="X9" t="n">
-        <v>0.197</v>
+        <v>0.196</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.444</v>
+        <v>0.443</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.393</v>
+        <v>0.392</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.239</v>
+        <v>0.238</v>
       </c>
       <c r="AB9" t="n">
         <v>0.488</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.341</v>
+        <v>0.342</v>
       </c>
       <c r="AD9" t="n">
         <v>0.225</v>
@@ -1939,61 +1939,61 @@
         <v>0.474</v>
       </c>
       <c r="AF9" t="n">
-        <v>0.209</v>
+        <v>0.208</v>
       </c>
       <c r="AG9" t="n">
         <v>0.165</v>
       </c>
       <c r="AH9" t="n">
-        <v>0.407</v>
+        <v>0.406</v>
       </c>
       <c r="AI9" t="n">
+        <v>0.278</v>
+      </c>
+      <c r="AJ9" t="n">
+        <v>0.201</v>
+      </c>
+      <c r="AK9" t="n">
+        <v>0.448</v>
+      </c>
+      <c r="AL9" t="n">
         <v>0.282</v>
       </c>
-      <c r="AJ9" t="n">
+      <c r="AM9" t="n">
         <v>0.203</v>
       </c>
-      <c r="AK9" t="n">
+      <c r="AN9" t="n">
         <v>0.45</v>
       </c>
-      <c r="AL9" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="AM9" t="n">
-        <v>0.202</v>
-      </c>
-      <c r="AN9" t="n">
-        <v>0.449</v>
-      </c>
       <c r="AO9" t="n">
-        <v>0.433</v>
+        <v>0.437</v>
       </c>
       <c r="AP9" t="n">
         <v>0.246</v>
       </c>
       <c r="AQ9" t="n">
-        <v>0.495</v>
+        <v>0.496</v>
       </c>
       <c r="AR9" t="n">
-        <v>0.207</v>
+        <v>0.208</v>
       </c>
       <c r="AS9" t="n">
-        <v>0.164</v>
+        <v>0.165</v>
       </c>
       <c r="AT9" t="n">
-        <v>0.405</v>
+        <v>0.406</v>
       </c>
       <c r="AU9" t="n">
-        <v>0.251</v>
+        <v>0.252</v>
       </c>
       <c r="AV9" t="n">
         <v>0.188</v>
       </c>
       <c r="AW9" t="n">
-        <v>0.433</v>
+        <v>0.434</v>
       </c>
       <c r="AX9" t="n">
-        <v>1.855</v>
+        <v>1.851</v>
       </c>
       <c r="AY9" t="n">
         <v>0.25</v>
@@ -2002,7 +2002,7 @@
         <v>0.5</v>
       </c>
       <c r="BA9" t="n">
-        <v>1.849</v>
+        <v>1.842</v>
       </c>
       <c r="BB9" t="n">
         <v>0.25</v>
@@ -2011,7 +2011,7 @@
         <v>0.5</v>
       </c>
       <c r="BD9" t="n">
-        <v>0.619</v>
+        <v>0.616</v>
       </c>
       <c r="BE9" t="n">
         <v>0.236</v>
@@ -2020,37 +2020,37 @@
         <v>0.486</v>
       </c>
       <c r="BG9" t="n">
-        <v>0.62</v>
+        <v>0.616</v>
       </c>
       <c r="BH9" t="n">
-        <v>0.236</v>
+        <v>0.237</v>
       </c>
       <c r="BI9" t="n">
-        <v>0.485</v>
+        <v>0.486</v>
       </c>
       <c r="BJ9" t="n">
-        <v>0.734</v>
+        <v>0.73</v>
       </c>
       <c r="BK9" t="n">
-        <v>0.195</v>
+        <v>0.197</v>
       </c>
       <c r="BL9" t="n">
-        <v>0.442</v>
+        <v>0.444</v>
       </c>
       <c r="BM9" t="n">
-        <v>0.728</v>
+        <v>0.722</v>
       </c>
       <c r="BN9" t="n">
-        <v>0.198</v>
+        <v>0.201</v>
       </c>
       <c r="BO9" t="n">
-        <v>0.445</v>
+        <v>0.448</v>
       </c>
       <c r="BP9" t="n">
-        <v>0.616</v>
+        <v>0.614</v>
       </c>
       <c r="BQ9" t="n">
-        <v>0.618</v>
+        <v>0.617</v>
       </c>
     </row>
     <row r="10">
@@ -2060,61 +2060,61 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.636</v>
+        <v>0.639</v>
       </c>
       <c r="C10" t="n">
-        <v>0.232</v>
+        <v>0.231</v>
       </c>
       <c r="D10" t="n">
-        <v>0.481</v>
+        <v>0.48</v>
       </c>
       <c r="E10" t="n">
-        <v>0.715</v>
+        <v>0.717</v>
       </c>
       <c r="F10" t="n">
-        <v>0.204</v>
+        <v>0.203</v>
       </c>
       <c r="G10" t="n">
         <v>0.451</v>
       </c>
       <c r="H10" t="n">
-        <v>0.709</v>
+        <v>0.711</v>
       </c>
       <c r="I10" t="n">
-        <v>0.206</v>
+        <v>0.205</v>
       </c>
       <c r="J10" t="n">
-        <v>0.454</v>
+        <v>0.453</v>
       </c>
       <c r="K10" t="n">
-        <v>0.77</v>
+        <v>0.773</v>
       </c>
       <c r="L10" t="n">
-        <v>0.177</v>
+        <v>0.175</v>
       </c>
       <c r="M10" t="n">
-        <v>0.421</v>
+        <v>0.419</v>
       </c>
       <c r="N10" t="n">
-        <v>0.887</v>
+        <v>0.888</v>
       </c>
       <c r="O10" t="n">
-        <v>0.101</v>
+        <v>0.099</v>
       </c>
       <c r="P10" t="n">
-        <v>0.317</v>
+        <v>0.315</v>
       </c>
       <c r="Q10" t="n">
         <v>0.026</v>
       </c>
       <c r="R10" t="n">
-        <v>0.026</v>
+        <v>0.025</v>
       </c>
       <c r="S10" t="n">
-        <v>0.16</v>
+        <v>0.159</v>
       </c>
       <c r="T10" t="n">
-        <v>0.448</v>
+        <v>0.447</v>
       </c>
       <c r="U10" t="n">
         <v>0.247</v>
@@ -2123,7 +2123,7 @@
         <v>0.497</v>
       </c>
       <c r="W10" t="n">
-        <v>0.406</v>
+        <v>0.405</v>
       </c>
       <c r="X10" t="n">
         <v>0.241</v>
@@ -2132,13 +2132,13 @@
         <v>0.491</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.611</v>
+        <v>0.606</v>
       </c>
       <c r="AA10" t="n">
-        <v>0.238</v>
+        <v>0.239</v>
       </c>
       <c r="AB10" t="n">
-        <v>0.488</v>
+        <v>0.489</v>
       </c>
       <c r="AC10" t="n">
         <v>0.379</v>
@@ -2150,7 +2150,7 @@
         <v>0.485</v>
       </c>
       <c r="AF10" t="n">
-        <v>0.314</v>
+        <v>0.313</v>
       </c>
       <c r="AG10" t="n">
         <v>0.215</v>
@@ -2159,10 +2159,10 @@
         <v>0.464</v>
       </c>
       <c r="AI10" t="n">
-        <v>0.393</v>
+        <v>0.39</v>
       </c>
       <c r="AJ10" t="n">
-        <v>0.239</v>
+        <v>0.238</v>
       </c>
       <c r="AK10" t="n">
         <v>0.488</v>
@@ -2177,13 +2177,13 @@
         <v>0.497</v>
       </c>
       <c r="AO10" t="n">
-        <v>0.573</v>
+        <v>0.577</v>
       </c>
       <c r="AP10" t="n">
-        <v>0.245</v>
+        <v>0.244</v>
       </c>
       <c r="AQ10" t="n">
-        <v>0.495</v>
+        <v>0.494</v>
       </c>
       <c r="AR10" t="n">
         <v>0.379</v>
@@ -2195,7 +2195,7 @@
         <v>0.485</v>
       </c>
       <c r="AU10" t="n">
-        <v>0.409</v>
+        <v>0.413</v>
       </c>
       <c r="AV10" t="n">
         <v>0.242</v>
@@ -2204,64 +2204,64 @@
         <v>0.492</v>
       </c>
       <c r="AX10" t="n">
-        <v>2.207</v>
+        <v>2.213</v>
       </c>
       <c r="AY10" t="n">
-        <v>0.234</v>
+        <v>0.232</v>
       </c>
       <c r="AZ10" t="n">
-        <v>0.483</v>
+        <v>0.482</v>
       </c>
       <c r="BA10" t="n">
-        <v>2.177</v>
+        <v>2.182</v>
       </c>
       <c r="BB10" t="n">
-        <v>0.237</v>
+        <v>0.235</v>
       </c>
       <c r="BC10" t="n">
-        <v>0.487</v>
+        <v>0.485</v>
       </c>
       <c r="BD10" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.6889999999999999</v>
       </c>
       <c r="BE10" t="n">
         <v>0.214</v>
       </c>
       <c r="BF10" t="n">
-        <v>0.462</v>
+        <v>0.463</v>
       </c>
       <c r="BG10" t="n">
-        <v>0.681</v>
+        <v>0.678</v>
       </c>
       <c r="BH10" t="n">
-        <v>0.217</v>
+        <v>0.218</v>
       </c>
       <c r="BI10" t="n">
-        <v>0.466</v>
+        <v>0.467</v>
       </c>
       <c r="BJ10" t="n">
-        <v>0.889</v>
+        <v>0.891</v>
       </c>
       <c r="BK10" t="n">
-        <v>0.099</v>
+        <v>0.097</v>
       </c>
       <c r="BL10" t="n">
-        <v>0.314</v>
+        <v>0.312</v>
       </c>
       <c r="BM10" t="n">
-        <v>0.881</v>
+        <v>0.883</v>
       </c>
       <c r="BN10" t="n">
-        <v>0.105</v>
+        <v>0.103</v>
       </c>
       <c r="BO10" t="n">
-        <v>0.323</v>
+        <v>0.321</v>
       </c>
       <c r="BP10" t="n">
-        <v>0.726</v>
+        <v>0.727</v>
       </c>
       <c r="BQ10" t="n">
-        <v>0.736</v>
+        <v>0.738</v>
       </c>
     </row>
     <row r="11">
@@ -2271,49 +2271,49 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.6820000000000001</v>
+        <v>0.6870000000000001</v>
       </c>
       <c r="C11" t="n">
-        <v>0.217</v>
+        <v>0.215</v>
       </c>
       <c r="D11" t="n">
-        <v>0.466</v>
+        <v>0.464</v>
       </c>
       <c r="E11" t="n">
-        <v>0.765</v>
+        <v>0.766</v>
       </c>
       <c r="F11" t="n">
-        <v>0.18</v>
+        <v>0.179</v>
       </c>
       <c r="G11" t="n">
-        <v>0.424</v>
+        <v>0.423</v>
       </c>
       <c r="H11" t="n">
-        <v>0.753</v>
+        <v>0.757</v>
       </c>
       <c r="I11" t="n">
-        <v>0.186</v>
+        <v>0.184</v>
       </c>
       <c r="J11" t="n">
-        <v>0.431</v>
+        <v>0.429</v>
       </c>
       <c r="K11" t="n">
-        <v>0.801</v>
+        <v>0.804</v>
       </c>
       <c r="L11" t="n">
-        <v>0.159</v>
+        <v>0.158</v>
       </c>
       <c r="M11" t="n">
-        <v>0.399</v>
+        <v>0.397</v>
       </c>
       <c r="N11" t="n">
-        <v>0.916</v>
+        <v>0.917</v>
       </c>
       <c r="O11" t="n">
-        <v>0.077</v>
+        <v>0.076</v>
       </c>
       <c r="P11" t="n">
-        <v>0.278</v>
+        <v>0.276</v>
       </c>
       <c r="Q11" t="n">
         <v>0.029</v>
@@ -2322,10 +2322,10 @@
         <v>0.028</v>
       </c>
       <c r="S11" t="n">
-        <v>0.168</v>
+        <v>0.167</v>
       </c>
       <c r="T11" t="n">
-        <v>0.45</v>
+        <v>0.449</v>
       </c>
       <c r="U11" t="n">
         <v>0.247</v>
@@ -2334,7 +2334,7 @@
         <v>0.497</v>
       </c>
       <c r="W11" t="n">
-        <v>0.406</v>
+        <v>0.405</v>
       </c>
       <c r="X11" t="n">
         <v>0.241</v>
@@ -2343,16 +2343,16 @@
         <v>0.491</v>
       </c>
       <c r="Z11" t="n">
-        <v>0.655</v>
+        <v>0.649</v>
       </c>
       <c r="AA11" t="n">
-        <v>0.226</v>
+        <v>0.228</v>
       </c>
       <c r="AB11" t="n">
-        <v>0.475</v>
+        <v>0.477</v>
       </c>
       <c r="AC11" t="n">
-        <v>0.383</v>
+        <v>0.384</v>
       </c>
       <c r="AD11" t="n">
         <v>0.236</v>
@@ -2361,25 +2361,25 @@
         <v>0.486</v>
       </c>
       <c r="AF11" t="n">
-        <v>0.335</v>
+        <v>0.334</v>
       </c>
       <c r="AG11" t="n">
-        <v>0.223</v>
+        <v>0.222</v>
       </c>
       <c r="AH11" t="n">
         <v>0.472</v>
       </c>
       <c r="AI11" t="n">
-        <v>0.42</v>
+        <v>0.416</v>
       </c>
       <c r="AJ11" t="n">
-        <v>0.244</v>
+        <v>0.243</v>
       </c>
       <c r="AK11" t="n">
         <v>0.493</v>
       </c>
       <c r="AL11" t="n">
-        <v>0.467</v>
+        <v>0.468</v>
       </c>
       <c r="AM11" t="n">
         <v>0.249</v>
@@ -2388,16 +2388,16 @@
         <v>0.499</v>
       </c>
       <c r="AO11" t="n">
-        <v>0.598</v>
+        <v>0.602</v>
       </c>
       <c r="AP11" t="n">
         <v>0.24</v>
       </c>
       <c r="AQ11" t="n">
-        <v>0.49</v>
+        <v>0.489</v>
       </c>
       <c r="AR11" t="n">
-        <v>0.469</v>
+        <v>0.47</v>
       </c>
       <c r="AS11" t="n">
         <v>0.249</v>
@@ -2406,7 +2406,7 @@
         <v>0.499</v>
       </c>
       <c r="AU11" t="n">
-        <v>0.504</v>
+        <v>0.509</v>
       </c>
       <c r="AV11" t="n">
         <v>0.25</v>
@@ -2415,64 +2415,64 @@
         <v>0.5</v>
       </c>
       <c r="AX11" t="n">
-        <v>2.221</v>
+        <v>2.227</v>
       </c>
       <c r="AY11" t="n">
-        <v>0.231</v>
+        <v>0.229</v>
       </c>
       <c r="AZ11" t="n">
-        <v>0.481</v>
+        <v>0.479</v>
       </c>
       <c r="BA11" t="n">
-        <v>2.187</v>
+        <v>2.193</v>
       </c>
       <c r="BB11" t="n">
-        <v>0.236</v>
+        <v>0.234</v>
       </c>
       <c r="BC11" t="n">
-        <v>0.485</v>
+        <v>0.484</v>
       </c>
       <c r="BD11" t="n">
-        <v>0.6919999999999999</v>
+        <v>0.6909999999999999</v>
       </c>
       <c r="BE11" t="n">
-        <v>0.213</v>
+        <v>0.214</v>
       </c>
       <c r="BF11" t="n">
-        <v>0.461</v>
+        <v>0.462</v>
       </c>
       <c r="BG11" t="n">
-        <v>0.6830000000000001</v>
+        <v>0.681</v>
       </c>
       <c r="BH11" t="n">
-        <v>0.216</v>
+        <v>0.217</v>
       </c>
       <c r="BI11" t="n">
-        <v>0.465</v>
+        <v>0.466</v>
       </c>
       <c r="BJ11" t="n">
-        <v>0.891</v>
+        <v>0.893</v>
       </c>
       <c r="BK11" t="n">
-        <v>0.097</v>
+        <v>0.096</v>
       </c>
       <c r="BL11" t="n">
-        <v>0.311</v>
+        <v>0.309</v>
       </c>
       <c r="BM11" t="n">
-        <v>0.884</v>
+        <v>0.886</v>
       </c>
       <c r="BN11" t="n">
-        <v>0.103</v>
+        <v>0.101</v>
       </c>
       <c r="BO11" t="n">
-        <v>0.32</v>
+        <v>0.318</v>
       </c>
       <c r="BP11" t="n">
-        <v>0.729</v>
+        <v>0.731</v>
       </c>
       <c r="BQ11" t="n">
-        <v>0.74</v>
+        <v>0.742</v>
       </c>
     </row>
     <row r="12">
@@ -2482,49 +2482,49 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1.583</v>
+        <v>1.604</v>
       </c>
       <c r="C12" t="n">
-        <v>0.9360000000000001</v>
+        <v>0.972</v>
       </c>
       <c r="D12" t="n">
-        <v>0.968</v>
+        <v>0.986</v>
       </c>
       <c r="E12" t="n">
-        <v>1.514</v>
+        <v>1.515</v>
       </c>
       <c r="F12" t="n">
-        <v>0.96</v>
+        <v>0.948</v>
       </c>
       <c r="G12" t="n">
-        <v>0.98</v>
+        <v>0.974</v>
       </c>
       <c r="H12" t="n">
-        <v>1.494</v>
+        <v>1.499</v>
       </c>
       <c r="I12" t="n">
-        <v>0.861</v>
+        <v>0.866</v>
       </c>
       <c r="J12" t="n">
-        <v>0.928</v>
+        <v>0.93</v>
       </c>
       <c r="K12" t="n">
-        <v>1.384</v>
+        <v>1.382</v>
       </c>
       <c r="L12" t="n">
-        <v>0.644</v>
+        <v>0.636</v>
       </c>
       <c r="M12" t="n">
-        <v>0.802</v>
+        <v>0.798</v>
       </c>
       <c r="N12" t="n">
-        <v>1.436</v>
+        <v>1.431</v>
       </c>
       <c r="O12" t="n">
-        <v>0.85</v>
+        <v>0.839</v>
       </c>
       <c r="P12" t="n">
-        <v>0.922</v>
+        <v>0.916</v>
       </c>
       <c r="Q12" t="n">
         <v>1.364</v>
@@ -2536,115 +2536,115 @@
         <v>0.881</v>
       </c>
       <c r="T12" t="n">
-        <v>1.419</v>
+        <v>1.417</v>
       </c>
       <c r="U12" t="n">
-        <v>0.439</v>
+        <v>0.436</v>
       </c>
       <c r="V12" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="W12" t="n">
+        <v>1.436</v>
+      </c>
+      <c r="X12" t="n">
+        <v>0.438</v>
+      </c>
+      <c r="Y12" t="n">
         <v>0.662</v>
       </c>
-      <c r="W12" t="n">
-        <v>1.429</v>
-      </c>
-      <c r="X12" t="n">
-        <v>0.427</v>
-      </c>
-      <c r="Y12" t="n">
-        <v>0.653</v>
-      </c>
       <c r="Z12" t="n">
-        <v>1.668</v>
+        <v>1.663</v>
       </c>
       <c r="AA12" t="n">
-        <v>0.931</v>
+        <v>0.928</v>
       </c>
       <c r="AB12" t="n">
-        <v>0.965</v>
+        <v>0.963</v>
       </c>
       <c r="AC12" t="n">
-        <v>1.137</v>
+        <v>1.134</v>
       </c>
       <c r="AD12" t="n">
-        <v>0.194</v>
+        <v>0.192</v>
       </c>
       <c r="AE12" t="n">
-        <v>0.441</v>
+        <v>0.438</v>
       </c>
       <c r="AF12" t="n">
-        <v>1.619</v>
+        <v>1.617</v>
       </c>
       <c r="AG12" t="n">
-        <v>0.923</v>
+        <v>0.915</v>
       </c>
       <c r="AH12" t="n">
-        <v>0.961</v>
+        <v>0.957</v>
       </c>
       <c r="AI12" t="n">
-        <v>1.637</v>
+        <v>1.64</v>
       </c>
       <c r="AJ12" t="n">
-        <v>1.119</v>
+        <v>1.112</v>
       </c>
       <c r="AK12" t="n">
-        <v>1.058</v>
+        <v>1.055</v>
       </c>
       <c r="AL12" t="n">
         <v>1.751</v>
       </c>
       <c r="AM12" t="n">
-        <v>1.619</v>
+        <v>1.62</v>
       </c>
       <c r="AN12" t="n">
         <v>1.273</v>
       </c>
       <c r="AO12" t="n">
-        <v>1.502</v>
+        <v>1.495</v>
       </c>
       <c r="AP12" t="n">
-        <v>1.018</v>
+        <v>1.003</v>
       </c>
       <c r="AQ12" t="n">
-        <v>1.009</v>
+        <v>1.001</v>
       </c>
       <c r="AR12" t="n">
-        <v>2.595</v>
+        <v>2.594</v>
       </c>
       <c r="AS12" t="n">
-        <v>3.261</v>
+        <v>3.253</v>
       </c>
       <c r="AT12" t="n">
-        <v>1.806</v>
+        <v>1.804</v>
       </c>
       <c r="AU12" t="n">
         <v>2.178</v>
       </c>
       <c r="AV12" t="n">
-        <v>2.227</v>
+        <v>2.206</v>
       </c>
       <c r="AW12" t="n">
-        <v>1.492</v>
+        <v>1.485</v>
       </c>
       <c r="AX12" t="n">
-        <v>3.643</v>
+        <v>3.649</v>
       </c>
       <c r="AY12" t="n">
-        <v>0.386</v>
+        <v>0.382</v>
       </c>
       <c r="AZ12" t="n">
-        <v>0.621</v>
+        <v>0.618</v>
       </c>
       <c r="BA12" t="n">
-        <v>3.595000000000001</v>
+        <v>3.607</v>
       </c>
       <c r="BB12" t="n">
-        <v>0.32</v>
+        <v>0.318</v>
       </c>
       <c r="BC12" t="n">
-        <v>0.5659999999999999</v>
+        <v>0.5639999999999999</v>
       </c>
       <c r="BD12" t="n">
-        <v>1.136</v>
+        <v>1.137</v>
       </c>
       <c r="BE12" t="n">
         <v>0.184</v>
@@ -2653,37 +2653,37 @@
         <v>0.429</v>
       </c>
       <c r="BG12" t="n">
-        <v>1.12</v>
+        <v>1.122</v>
       </c>
       <c r="BH12" t="n">
-        <v>0.167</v>
+        <v>0.168</v>
       </c>
       <c r="BI12" t="n">
-        <v>0.409</v>
+        <v>0.41</v>
       </c>
       <c r="BJ12" t="n">
-        <v>1.225</v>
+        <v>1.23</v>
       </c>
       <c r="BK12" t="n">
-        <v>0.301</v>
+        <v>0.302</v>
       </c>
       <c r="BL12" t="n">
-        <v>0.548</v>
+        <v>0.549</v>
       </c>
       <c r="BM12" t="n">
-        <v>1.232</v>
+        <v>1.24</v>
       </c>
       <c r="BN12" t="n">
-        <v>0.327</v>
+        <v>0.328</v>
       </c>
       <c r="BO12" t="n">
-        <v>0.572</v>
+        <v>0.573</v>
       </c>
       <c r="BP12" t="n">
-        <v>1.198</v>
+        <v>1.202</v>
       </c>
       <c r="BQ12" t="n">
-        <v>1.214</v>
+        <v>1.216</v>
       </c>
     </row>
     <row r="13">
@@ -2693,49 +2693,49 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1.458</v>
+        <v>1.457</v>
       </c>
       <c r="C13" t="n">
-        <v>0.355</v>
+        <v>0.354</v>
       </c>
       <c r="D13" t="n">
-        <v>0.596</v>
+        <v>0.595</v>
       </c>
       <c r="E13" t="n">
-        <v>1.58</v>
+        <v>1.577</v>
       </c>
       <c r="F13" t="n">
-        <v>0.465</v>
+        <v>0.462</v>
       </c>
       <c r="G13" t="n">
-        <v>0.6820000000000001</v>
+        <v>0.68</v>
       </c>
       <c r="H13" t="n">
         <v>1.776</v>
       </c>
       <c r="I13" t="n">
-        <v>0.466</v>
+        <v>0.463</v>
       </c>
       <c r="J13" t="n">
-        <v>0.6830000000000001</v>
+        <v>0.68</v>
       </c>
       <c r="K13" t="n">
         <v>1.78</v>
       </c>
       <c r="L13" t="n">
-        <v>0.456</v>
+        <v>0.453</v>
       </c>
       <c r="M13" t="n">
-        <v>0.675</v>
+        <v>0.673</v>
       </c>
       <c r="N13" t="n">
-        <v>2.078</v>
+        <v>2.076</v>
       </c>
       <c r="O13" t="n">
-        <v>1.065</v>
+        <v>1.057</v>
       </c>
       <c r="P13" t="n">
-        <v>1.032</v>
+        <v>1.028</v>
       </c>
       <c r="Q13" t="n">
         <v>0.529</v>
@@ -2747,16 +2747,16 @@
         <v>0.279</v>
       </c>
       <c r="T13" t="n">
-        <v>0.985</v>
+        <v>0.982</v>
       </c>
       <c r="U13" t="n">
-        <v>0.179</v>
+        <v>0.178</v>
       </c>
       <c r="V13" t="n">
-        <v>0.423</v>
+        <v>0.422</v>
       </c>
       <c r="W13" t="n">
-        <v>1.057</v>
+        <v>1.055</v>
       </c>
       <c r="X13" t="n">
         <v>0.211</v>
@@ -2765,136 +2765,136 @@
         <v>0.459</v>
       </c>
       <c r="Z13" t="n">
-        <v>1.515</v>
+        <v>1.511</v>
       </c>
       <c r="AA13" t="n">
-        <v>0.316</v>
+        <v>0.314</v>
       </c>
       <c r="AB13" t="n">
-        <v>0.5620000000000001</v>
+        <v>0.5610000000000001</v>
       </c>
       <c r="AC13" t="n">
+        <v>0.555</v>
+      </c>
+      <c r="AD13" t="n">
+        <v>0.097</v>
+      </c>
+      <c r="AE13" t="n">
+        <v>0.312</v>
+      </c>
+      <c r="AF13" t="n">
+        <v>1.141</v>
+      </c>
+      <c r="AG13" t="n">
+        <v>0.332</v>
+      </c>
+      <c r="AH13" t="n">
+        <v>0.576</v>
+      </c>
+      <c r="AI13" t="n">
+        <v>1.291</v>
+      </c>
+      <c r="AJ13" t="n">
+        <v>0.326</v>
+      </c>
+      <c r="AK13" t="n">
+        <v>0.571</v>
+      </c>
+      <c r="AL13" t="n">
+        <v>1.537</v>
+      </c>
+      <c r="AM13" t="n">
+        <v>0.826</v>
+      </c>
+      <c r="AN13" t="n">
+        <v>0.909</v>
+      </c>
+      <c r="AO13" t="n">
+        <v>1.147</v>
+      </c>
+      <c r="AP13" t="n">
+        <v>0.784</v>
+      </c>
+      <c r="AQ13" t="n">
+        <v>0.886</v>
+      </c>
+      <c r="AR13" t="n">
+        <v>2.785</v>
+      </c>
+      <c r="AS13" t="n">
+        <v>1.348</v>
+      </c>
+      <c r="AT13" t="n">
+        <v>1.161</v>
+      </c>
+      <c r="AU13" t="n">
+        <v>2.305</v>
+      </c>
+      <c r="AV13" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="AW13" t="n">
+        <v>0.877</v>
+      </c>
+      <c r="AX13" t="n">
+        <v>2.246</v>
+      </c>
+      <c r="AY13" t="n">
+        <v>0.246</v>
+      </c>
+      <c r="AZ13" t="n">
+        <v>0.496</v>
+      </c>
+      <c r="BA13" t="n">
+        <v>2.366</v>
+      </c>
+      <c r="BB13" t="n">
+        <v>0.273</v>
+      </c>
+      <c r="BC13" t="n">
+        <v>0.522</v>
+      </c>
+      <c r="BD13" t="n">
         <v>0.556</v>
-      </c>
-      <c r="AD13" t="n">
-        <v>0.098</v>
-      </c>
-      <c r="AE13" t="n">
-        <v>0.313</v>
-      </c>
-      <c r="AF13" t="n">
-        <v>1.145</v>
-      </c>
-      <c r="AG13" t="n">
-        <v>0.328</v>
-      </c>
-      <c r="AH13" t="n">
-        <v>0.572</v>
-      </c>
-      <c r="AI13" t="n">
-        <v>1.29</v>
-      </c>
-      <c r="AJ13" t="n">
-        <v>0.323</v>
-      </c>
-      <c r="AK13" t="n">
-        <v>0.569</v>
-      </c>
-      <c r="AL13" t="n">
-        <v>1.526</v>
-      </c>
-      <c r="AM13" t="n">
-        <v>0.8090000000000001</v>
-      </c>
-      <c r="AN13" t="n">
-        <v>0.899</v>
-      </c>
-      <c r="AO13" t="n">
-        <v>1.151</v>
-      </c>
-      <c r="AP13" t="n">
-        <v>0.788</v>
-      </c>
-      <c r="AQ13" t="n">
-        <v>0.888</v>
-      </c>
-      <c r="AR13" t="n">
-        <v>2.782</v>
-      </c>
-      <c r="AS13" t="n">
-        <v>1.36</v>
-      </c>
-      <c r="AT13" t="n">
-        <v>1.166</v>
-      </c>
-      <c r="AU13" t="n">
-        <v>2.308</v>
-      </c>
-      <c r="AV13" t="n">
-        <v>0.773</v>
-      </c>
-      <c r="AW13" t="n">
-        <v>0.879</v>
-      </c>
-      <c r="AX13" t="n">
-        <v>2.252</v>
-      </c>
-      <c r="AY13" t="n">
-        <v>0.249</v>
-      </c>
-      <c r="AZ13" t="n">
-        <v>0.499</v>
-      </c>
-      <c r="BA13" t="n">
-        <v>2.373</v>
-      </c>
-      <c r="BB13" t="n">
-        <v>0.276</v>
-      </c>
-      <c r="BC13" t="n">
-        <v>0.525</v>
-      </c>
-      <c r="BD13" t="n">
-        <v>0.5570000000000001</v>
       </c>
       <c r="BE13" t="n">
         <v>0.074</v>
       </c>
       <c r="BF13" t="n">
-        <v>0.273</v>
+        <v>0.272</v>
       </c>
       <c r="BG13" t="n">
-        <v>0.583</v>
+        <v>0.582</v>
       </c>
       <c r="BH13" t="n">
-        <v>0.094</v>
+        <v>0.093</v>
       </c>
       <c r="BI13" t="n">
-        <v>0.306</v>
+        <v>0.305</v>
       </c>
       <c r="BJ13" t="n">
-        <v>0.846</v>
+        <v>0.845</v>
       </c>
       <c r="BK13" t="n">
-        <v>0.199</v>
+        <v>0.197</v>
       </c>
       <c r="BL13" t="n">
-        <v>0.446</v>
+        <v>0.443</v>
       </c>
       <c r="BM13" t="n">
-        <v>0.914</v>
+        <v>0.912</v>
       </c>
       <c r="BN13" t="n">
-        <v>0.242</v>
+        <v>0.239</v>
       </c>
       <c r="BO13" t="n">
-        <v>0.492</v>
+        <v>0.489</v>
       </c>
       <c r="BP13" t="n">
-        <v>0.791</v>
+        <v>0.789</v>
       </c>
       <c r="BQ13" t="n">
-        <v>0.751</v>
+        <v>0.749</v>
       </c>
     </row>
   </sheetData>

</xml_diff>